<commit_message>
Update Glosario Data Climático.xlsx
</commit_message>
<xml_diff>
--- a/CHILE/00 Causas Antropógenas/Glosario Data Climático.xlsx
+++ b/CHILE/00 Causas Antropógenas/Glosario Data Climático.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gustavo Arancibia\Dropbox\Diseño DATA's (1)\DATA-ICC\CHILE\00 Causas Antropógenas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C911F43-EDF8-49E3-A6AE-291D5B49EBDF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FA61985-A594-445D-8C68-6E5FEF88AFF3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{60F8DE14-65AF-4259-A23A-4471DDD3B515}"/>
   </bookViews>
@@ -33,15 +33,9 @@
     <t>GEI</t>
   </si>
   <si>
-    <t xml:space="preserve"> gas de efecto invernadero. Es un gas atmosférico que emite y absorbe radiación dentro del rango infrarrojo, lo cual es una de las principales causas del efecto invernadero.</t>
-  </si>
-  <si>
     <t>CO2</t>
   </si>
   <si>
-    <t xml:space="preserve"> el dióxido de carbono es un gas de origen natural y un subproducto de la combustión de combustibles fósiles, como el petróleo, el carbón o el gas, de la quema de biomasa, y de los cambios de uso del suelo y otros procesos industriales, como en la producción de cemento. Es el principal gas de efecto invernadero antropógeno por lo que es usado como referencia para medir otros gases de efecto invernadero. Su potencial de calentamiento global es igual a 1.</t>
-  </si>
-  <si>
     <t>N2O</t>
   </si>
   <si>
@@ -54,39 +48,24 @@
     <t>SF6</t>
   </si>
   <si>
-    <t xml:space="preserve"> el hexafluoruro de azufre es un gas artificial inerte y neutro. Es un muy buen aislante eléctrico y tiene gran capacidad calórica. Su vida media se estima en 3.200 años convirtiéndose en un producto no degradable. Su potencial de calentamiento global es de 22.800, por lo que sólo 1 kg de SF6 equivale a casi 24 toneladas de CO2. </t>
-  </si>
-  <si>
     <t>CO2e</t>
   </si>
   <si>
     <t>PIB</t>
   </si>
   <si>
-    <t xml:space="preserve"> el producto interno bruto es un indicador económico que refleja el valor monetario de todos los bienes y servicios finales producidos por un país en un periodo de tiempo, normalmente un año. Este indicador es usado para medir la riqueza generada por el país.</t>
-  </si>
-  <si>
     <t>Intensidad de la Energía</t>
   </si>
   <si>
-    <t xml:space="preserve"> es una medida que permite calcular la cantidad de recursos energéticos necesarios para que un país pueda generar su PIB.</t>
-  </si>
-  <si>
     <t>Intensidad del Carbono</t>
   </si>
   <si>
-    <t xml:space="preserve"> es una medida de cuánto CO2 se emite por kilowatt-hora de electricidad consumida.</t>
-  </si>
-  <si>
     <t>Agricultura</t>
   </si>
   <si>
     <t>Energía</t>
   </si>
   <si>
-    <t xml:space="preserve"> este sector incluye el consumo/quema de combustibles fósiles en el país y las emisiones fugitivas asociadas, que son todas las emisiones intencionales o no intencionales de gases de efecto invernadero emitidas durante la extracción, procesamiento, almacenamiento y distribución de combustibles fósiles.</t>
-  </si>
-  <si>
     <t>Procesos Industriales</t>
   </si>
   <si>
@@ -99,42 +78,12 @@
     <t>Emisiones Netas</t>
   </si>
   <si>
-    <t xml:space="preserve"> es la sumatoria de las emisiones y absorciones de los gases de efecto invernadero, también se entiende como "balance".</t>
-  </si>
-  <si>
     <t>Emisiones Netas per cápita</t>
   </si>
   <si>
-    <t xml:space="preserve"> son las emisiones netas emitidas por cada persona en el país de acuerdo al año de referencia.</t>
-  </si>
-  <si>
     <t>Emisiones Totales</t>
   </si>
   <si>
-    <t xml:space="preserve"> contabiliza solo a las emisiones de gases de efecto invernadero.</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> el óxido nitroso es un gas incoloro y no inflamable Este gas es producido naturalmente por bacterias. Por otro lado, se produce de manera antropogénica en el sector ganadero y en la industria. En la atmósfera se comporta como un gas de efecto invernadero con un potencial de calentamiento global de 298.</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> el metano es un gas incoloro, inflamable y no tóxico. Este gas se produce naturalmente por medio de la descomposición de materia orgánica. Las principales fuentes de emisión de metano a la atmósfera son el ganado, la energía y los humedales. Actúa como gas de efecto invernadero con un potencial de calentamiento global de 25.</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> el CO2 “equivalente” permite expresar el nivel de calentamiento global de los gases de efecto invernadero en términos del CO2 . Por ejemplo, 1 tonelada de CH4 es equivalente a 25 toneladas de CO2e.</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> este sector incluye las emisiones de gases de efecto invernadero asociadas a las actividades agropecuarias, tales como fermentación entérica, gestión de estiércol, cultivo de arroz, suelos agrícolas, quema de residuos agrícolas en el campo, encalado y aplicación de urea.</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> este sector  incluye las emisiones de gases de efecto invernadero producidas por diferentes actividades industriales que transforman materias primas, ya sea por medios químicos o físicos. Estas industrias contemplan a la industria de los minerales, industria química, industria de los metales, productos no energéticos de combustibles y uso de solventes, uso de produtos como sustitutos de las sustancias que agotan la capa de ozono y, manufacturas y utilización de otros productos.</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> este sector  incluye las emisiones de gases de efecto invernadero producidas por procesos microbiológicos que ocurren en la materia orgánica de residuos sólidos bajo degradación anaeróbica y por el tratamiento anaeróbico de aguas residuales industriales y domésticas. Las actividades emisoras principales son la disposición de residuos sólidos, el tratamiento biológico de residuos sólidos, la incineración y quema abierta de residuos, y el tratamiento y descarga de aguas residuales.</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> se define como "usos de la tierra, cambios en el uso de la tierra, y silvicultura". Este sector incluye las emisiones y absorciones de gases de efecto invernadero relacionadas a actividades silvícolas y al cambio de uso de la tierra. Dentro de los cambios de uso se encuentran: tierras forestales, tierras de cultivo, pastizales, humedales, asentamientos y otras tierras (zonas de suelo desnudo, roca, hielo y todas las zonas de tierras no gestionadas).</t>
-  </si>
-  <si>
     <t>Concepto</t>
   </si>
   <si>
@@ -156,7 +105,58 @@
     <t>Sectores</t>
   </si>
   <si>
-    <t xml:space="preserve"> los hidrofluorocarbonos son gases refrigerantes. La presencia de flúor en su composición hace que se comporten como un gas de efecto invernadero, contribuyendo al calentamiento global. El potencial de calentamiento global de los HFC rondan entre 124 y 14.800.</t>
+    <t xml:space="preserve"> Gas de efecto invernadero. Es un gas atmosférico que emite y absorbe radiación dentro del rango infrarrojo, lo cual es una de las principales causas del efecto invernadero.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> El dióxido de carbono es un gas de origen natural y un subproducto de la combustión de combustibles fósiles, como el petróleo, el carbón o el gas, de la quema de biomasa, y de los cambios de uso del suelo y otros procesos industriales, como en la producción de cemento. Es el principal gas de efecto invernadero antropógeno por lo que es usado como referencia para medir otros gases de efecto invernadero. Su potencial de calentamiento global es igual a 1.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> El óxido nitroso es un gas incoloro y no inflamable Este gas es producido naturalmente por bacterias. Por otro lado, se produce de manera antropogénica en el sector ganadero y en la industria. En la atmósfera se comporta como un gas de efecto invernadero con un potencial de calentamiento global de 298.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> El metano es un gas incoloro, inflamable y no tóxico. Este gas se produce naturalmente por medio de la descomposición de materia orgánica. Las principales fuentes de emisión de metano a la atmósfera son el ganado, la energía y los humedales. Actúa como gas de efecto invernadero con un potencial de calentamiento global de 25.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Los hidrofluorocarbonos son gases refrigerantes. La presencia de flúor en su composición hace que se comporten como un gas de efecto invernadero, contribuyendo al calentamiento global. El potencial de calentamiento global de los HFC rondan entre 124 y 14.800.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> El hexafluoruro de azufre es un gas artificial inerte y neutro. Es un muy buen aislante eléctrico y tiene gran capacidad calórica. Su vida media se estima en 3.200 años convirtiéndose en un producto no degradable. Su potencial de calentamiento global es de 22.800, por lo que sólo 1 kg de SF6 equivale a casi 24 toneladas de CO2. </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> El CO2 “equivalente” permite expresar el nivel de calentamiento global de los gases de efecto invernadero en términos del CO2 . Por ejemplo, 1 tonelada de CH4 es equivalente a 25 toneladas de CO2e.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> El producto interno bruto es un indicador económico que refleja el valor monetario de todos los bienes y servicios finales producidos por un país en un periodo de tiempo, normalmente un año. Este indicador es usado para medir la riqueza generada por el país.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Es una medida que permite calcular la cantidad de recursos energéticos necesarios para que un país pueda generar su PIB.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Es una medida de cuánto CO2 se emite por kilowatt-hora de electricidad consumida.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Este sector incluye las emisiones de gases de efecto invernadero asociadas a las actividades agropecuarias, tales como fermentación entérica, gestión de estiércol, cultivo de arroz, suelos agrícolas, quema de residuos agrícolas en el campo, encalado y aplicación de urea.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Este sector incluye el consumo/quema de combustibles fósiles en el país y las emisiones fugitivas asociadas, que son todas las emisiones intencionales o no intencionales de gases de efecto invernadero emitidas durante la extracción, procesamiento, almacenamiento y distribución de combustibles fósiles.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Este sector  incluye las emisiones de gases de efecto invernadero producidas por diferentes actividades industriales que transforman materias primas, ya sea por medios químicos o físicos. Estas industrias contemplan a la industria de los minerales, industria química, industria de los metales, productos no energéticos de combustibles y uso de solventes, uso de produtos como sustitutos de las sustancias que agotan la capa de ozono y, manufacturas y utilización de otros productos.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Este sector  incluye las emisiones de gases de efecto invernadero producidas por procesos microbiológicos que ocurren en la materia orgánica de residuos sólidos bajo degradación anaeróbica y por el tratamiento anaeróbico de aguas residuales industriales y domésticas. Las actividades emisoras principales son la disposición de residuos sólidos, el tratamiento biológico de residuos sólidos, la incineración y quema abierta de residuos, y el tratamiento y descarga de aguas residuales.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Se define como "usos de la tierra, cambios en el uso de la tierra, y silvicultura". Este sector incluye las emisiones y absorciones de gases de efecto invernadero relacionadas a actividades silvícolas y al cambio de uso de la tierra. Dentro de los cambios de uso se encuentran: tierras forestales, tierras de cultivo, pastizales, humedales, asentamientos y otras tierras (zonas de suelo desnudo, roca, hielo y todas las zonas de tierras no gestionadas).</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Es la sumatoria de las emisiones y absorciones de los gases de efecto invernadero, también se entiende como "balance".</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Son las emisiones netas emitidas por cada persona en el país de acuerdo al año de referencia.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Contabiliza solo a las emisiones de gases de efecto invernadero.</t>
   </si>
 </sst>
 </file>
@@ -538,7 +538,7 @@
   <dimension ref="A1:C21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -556,211 +556,211 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>38</v>
+        <v>21</v>
       </c>
       <c r="B3" t="s">
-        <v>36</v>
+        <v>19</v>
       </c>
       <c r="C3" t="s">
-        <v>37</v>
+        <v>20</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>39</v>
+        <v>22</v>
       </c>
       <c r="B4" t="s">
         <v>1</v>
       </c>
       <c r="C4" t="s">
-        <v>2</v>
+        <v>26</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>41</v>
+        <v>24</v>
       </c>
       <c r="B5" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C5" t="s">
-        <v>4</v>
+        <v>27</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>41</v>
+        <v>24</v>
       </c>
       <c r="B6" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C6" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>41</v>
+        <v>24</v>
       </c>
       <c r="B7" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C7" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>41</v>
+        <v>24</v>
       </c>
       <c r="B8" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C8" t="s">
-        <v>43</v>
+        <v>30</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>41</v>
+        <v>24</v>
       </c>
       <c r="B9" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C9" t="s">
-        <v>9</v>
+        <v>31</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>41</v>
+        <v>24</v>
       </c>
       <c r="B10" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C10" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>40</v>
+        <v>23</v>
       </c>
       <c r="B11" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="C11" t="s">
-        <v>12</v>
+        <v>33</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>40</v>
+        <v>23</v>
       </c>
       <c r="B12" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C12" t="s">
-        <v>14</v>
+        <v>34</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>40</v>
+        <v>23</v>
       </c>
       <c r="B13" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="C13" t="s">
-        <v>16</v>
+        <v>35</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>42</v>
+        <v>25</v>
       </c>
       <c r="B14" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="C14" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>42</v>
+        <v>25</v>
       </c>
       <c r="B15" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="C15" t="s">
-        <v>19</v>
+        <v>37</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>42</v>
+        <v>25</v>
       </c>
       <c r="B16" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="C16" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>42</v>
+        <v>25</v>
       </c>
       <c r="B17" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="C17" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>42</v>
+        <v>25</v>
       </c>
       <c r="B18" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="C18" t="s">
-        <v>35</v>
+        <v>40</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>39</v>
+        <v>22</v>
       </c>
       <c r="B19" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="C19" t="s">
-        <v>24</v>
+        <v>41</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>39</v>
+        <v>22</v>
       </c>
       <c r="B20" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="C20" t="s">
-        <v>26</v>
+        <v>42</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>39</v>
+        <v>22</v>
       </c>
       <c r="B21" t="s">
-        <v>27</v>
+        <v>18</v>
       </c>
       <c r="C21" t="s">
-        <v>28</v>
+        <v>43</v>
       </c>
     </row>
   </sheetData>

</xml_diff>